<commit_message>
update slinky with notes
</commit_message>
<xml_diff>
--- a/Data/PositionalData.xlsx
+++ b/Data/PositionalData.xlsx
@@ -78,6 +78,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="170" formatCode="0.0000000"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -143,10 +146,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -156,8 +161,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -699,18 +704,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="4" t="s">
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
@@ -1020,35 +1025,41 @@
   <dimension ref="A1:M13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K23" sqref="K23"/>
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="3" width="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="7" width="9.36328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="10" bestFit="1" customWidth="1"/>
+    <col min="10" max="13" width="9.36328125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5" t="s">
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5" t="s">
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5" t="s">
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="L1" s="5"/>
-      <c r="M1" s="5"/>
+      <c r="L1" s="7"/>
+      <c r="M1" s="7"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
@@ -1092,40 +1103,40 @@
       <c r="A3">
         <v>1</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="8">
         <v>4.4838049631009139E-2</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="8">
         <v>-1.2444450091784687E-2</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="8">
         <v>0.49629886842322057</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="8">
         <v>3.1946146469902763E-4</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="8">
         <v>1.092997643258612E-3</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="8">
         <v>4.6040194339480665E-4</v>
       </c>
-      <c r="H3">
+      <c r="H3" s="8">
         <v>4.7128003390356034E-2</v>
       </c>
-      <c r="I3">
+      <c r="I3" s="8">
         <v>4.3057435545428041E-2</v>
       </c>
-      <c r="J3">
+      <c r="J3" s="8">
         <v>0.5267701313413421</v>
       </c>
-      <c r="K3">
+      <c r="K3" s="8">
         <v>2.9726696467664612E-2</v>
       </c>
-      <c r="L3">
+      <c r="L3" s="8">
         <v>2.1784125102399715E-2</v>
       </c>
-      <c r="M3">
+      <c r="M3" s="8">
         <v>0.2744238391233364</v>
       </c>
     </row>
@@ -1133,40 +1144,40 @@
       <c r="A4">
         <v>2</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="8">
         <v>4.5656902249902452E-2</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="8">
         <v>0.14071060810238115</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="8">
         <v>0.49881251466770954</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="8">
         <v>1.7248181035309797E-3</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="8">
         <v>1.7669224379781585E-3</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="8">
         <v>5.7078283970153371E-4</v>
       </c>
-      <c r="H4">
+      <c r="H4" s="8">
         <v>4.523517051711675E-2</v>
       </c>
-      <c r="I4">
+      <c r="I4" s="8">
         <v>-1.2105281891611669E-2</v>
       </c>
-      <c r="J4">
+      <c r="J4" s="8">
         <v>0.49633335073788931</v>
       </c>
-      <c r="K4">
+      <c r="K4" s="8">
         <v>1.6917180941669419E-3</v>
       </c>
-      <c r="L4">
+      <c r="L4" s="8">
         <v>8.3585617229164097E-4</v>
       </c>
-      <c r="M4">
+      <c r="M4" s="8">
         <v>4.7638693396871967E-4</v>
       </c>
     </row>
@@ -1174,40 +1185,40 @@
       <c r="A5">
         <v>3</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="8">
         <v>5.1558875382460387E-2</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="8">
         <v>-1.8775157919474712E-2</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="8">
         <v>0.30000001192092773</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="8">
         <v>2.4704801001487796E-4</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="8">
         <v>4.9409675376161906E-4</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="8">
         <v>2.7997986992107904E-16</v>
       </c>
-      <c r="H5">
+      <c r="H5" s="8">
         <v>5.8920118957757943E-2</v>
       </c>
-      <c r="I5">
+      <c r="I5" s="8">
         <v>7.64049797736365E-2</v>
       </c>
-      <c r="J5">
+      <c r="J5" s="8">
         <v>0.29900002479553217</v>
       </c>
-      <c r="K5">
+      <c r="K5" s="8">
         <v>4.1996980488161851E-17</v>
       </c>
-      <c r="L5">
+      <c r="L5" s="8">
         <v>1.5977045417069226E-4</v>
       </c>
-      <c r="M5">
+      <c r="M5" s="8">
         <v>1.6798792195264741E-16</v>
       </c>
     </row>
@@ -1215,40 +1226,40 @@
       <c r="A6">
         <v>4</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="8">
         <v>-5.4794640047475689E-2</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="8">
         <v>0.13563514524139461</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="8">
         <v>0.49642189126461728</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="8">
         <v>5.1543720414366171E-4</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="8">
         <v>5.9687031636326826E-4</v>
       </c>
-      <c r="G6">
+      <c r="G6" s="8">
         <v>4.9775644381397529E-4</v>
       </c>
-      <c r="H6">
+      <c r="H6" s="8">
         <v>-5.5095032206736491E-2</v>
       </c>
-      <c r="I6">
+      <c r="I6" s="8">
         <v>-9.2284737038426084E-3</v>
       </c>
-      <c r="J6">
+      <c r="J6" s="8">
         <v>0.49973437841981649</v>
       </c>
-      <c r="K6">
+      <c r="K6" s="8">
         <v>4.9076877016915297E-5</v>
       </c>
-      <c r="L6">
+      <c r="L6" s="8">
         <v>8.2203851920232068E-6</v>
       </c>
-      <c r="M6">
+      <c r="M6" s="8">
         <v>4.4515118778826055E-4</v>
       </c>
     </row>
@@ -1256,40 +1267,40 @@
       <c r="A7">
         <v>5</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="8">
         <v>-5.4160260068981537E-2</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="8">
         <v>1.2509155988126429E-3</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="8">
         <v>0.79421017394549598</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="8">
         <v>1.552272344765385E-3</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="8">
         <v>7.5473254458889236E-3</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="8">
         <v>1.4268105931521577E-3</v>
       </c>
-      <c r="H7">
+      <c r="H7" s="8">
         <v>-5.2682869487266609E-2</v>
       </c>
-      <c r="I7">
+      <c r="I7" s="8">
         <v>0.14658575019110789</v>
       </c>
-      <c r="J7">
+      <c r="J7" s="8">
         <v>0.79622468784235512</v>
       </c>
-      <c r="K7">
+      <c r="K7" s="8">
         <v>1.1941387262985911E-3</v>
       </c>
-      <c r="L7">
+      <c r="L7" s="8">
         <v>1.215931567573383E-3</v>
       </c>
-      <c r="M7">
+      <c r="M7" s="8">
         <v>8.5451638172360719E-4</v>
       </c>
     </row>
@@ -1297,40 +1308,40 @@
       <c r="A8">
         <v>6</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="8">
         <v>0.23259794984299387</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="8">
         <v>-1.0278330175564183E-2</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="8">
         <v>0.50244233585320985</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="8">
         <v>1.347053621126659E-3</v>
       </c>
-      <c r="F8">
+      <c r="F8" s="8">
         <v>9.5208405436296494E-4</v>
       </c>
-      <c r="G8">
+      <c r="G8" s="8">
         <v>5.5435636690753982E-4</v>
       </c>
-      <c r="H8">
+      <c r="H8" s="8">
         <v>0.23100300376804972</v>
       </c>
-      <c r="I8">
+      <c r="I8" s="8">
         <v>0.14184857990879235</v>
       </c>
-      <c r="J8">
+      <c r="J8" s="8">
         <v>0.50574041616458143</v>
       </c>
-      <c r="K8">
+      <c r="K8" s="8">
         <v>1.0784327845595825E-3</v>
       </c>
-      <c r="L8">
+      <c r="L8" s="8">
         <v>1.5135326130162458E-4</v>
       </c>
-      <c r="M8">
+      <c r="M8" s="8">
         <v>5.3961697597610183E-4</v>
       </c>
     </row>
@@ -1338,40 +1349,40 @@
       <c r="A9">
         <v>7</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="8">
         <v>0.21914483673042701</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="8">
         <v>-1.317119319897349E-2</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="8">
         <v>0.75725559128655329</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="8">
         <v>5.6642760844778112E-3</v>
       </c>
-      <c r="F9">
+      <c r="F9" s="8">
         <v>2.7936871265328918E-3</v>
       </c>
-      <c r="G9">
+      <c r="G9" s="8">
         <v>1.9030178968982465E-2</v>
       </c>
-      <c r="H9">
+      <c r="H9" s="8">
         <v>0.23793984651565528</v>
       </c>
-      <c r="I9">
+      <c r="I9" s="8">
         <v>0.14438967472977046</v>
       </c>
-      <c r="J9">
+      <c r="J9" s="8">
         <v>0.80120002826054892</v>
       </c>
-      <c r="K9">
+      <c r="K9" s="8">
         <v>1.4686657622936612E-3</v>
       </c>
-      <c r="L9">
+      <c r="L9" s="8">
         <v>1.8400196952795057E-3</v>
       </c>
-      <c r="M9">
+      <c r="M9" s="8">
         <v>2.5756044927273823E-3</v>
       </c>
     </row>
@@ -1379,163 +1390,163 @@
       <c r="A10">
         <v>8</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="8">
         <v>0.13900677142840476</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="8">
         <v>-1.911669554856588E-2</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="8">
         <v>0.29657548525423366</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="8">
         <v>4.5092484326699384E-4</v>
       </c>
-      <c r="F10">
+      <c r="F10" s="8">
         <v>4.2820574703077526E-4</v>
       </c>
-      <c r="G10">
+      <c r="G10" s="8">
         <v>4.9662770525292857E-4</v>
       </c>
-      <c r="H10">
+      <c r="H10" s="8">
         <v>0.1381532102823253</v>
       </c>
-      <c r="I10">
+      <c r="I10" s="8">
         <v>2.9180398070306139E-2</v>
       </c>
-      <c r="J10">
+      <c r="J10" s="8">
         <v>0.29600000381469721</v>
       </c>
-      <c r="K10">
+      <c r="K10" s="8">
         <v>3.0676175006306604E-16</v>
       </c>
-      <c r="L10">
+      <c r="L10" s="8">
         <v>6.0102496092286752E-5</v>
       </c>
-      <c r="M10">
+      <c r="M10" s="8">
         <v>2.2309945459132076E-16</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A11" s="6">
+      <c r="A11" s="3">
         <v>9</v>
       </c>
-      <c r="B11" s="6">
+      <c r="B11" s="9">
         <v>0.14716587960720023</v>
       </c>
-      <c r="C11" s="6">
+      <c r="C11" s="9">
         <v>7.1445235516875971E-4</v>
       </c>
-      <c r="D11" s="6">
+      <c r="D11" s="9">
         <v>0.29300001263618447</v>
       </c>
-      <c r="E11" s="6">
+      <c r="E11" s="9">
         <v>2.2316322462394835E-16</v>
       </c>
-      <c r="F11" s="6">
+      <c r="F11" s="9">
         <v>7.6276492791388599E-19</v>
       </c>
-      <c r="G11" s="6">
+      <c r="G11" s="9">
         <v>4.463264492478967E-16</v>
       </c>
-      <c r="H11" s="6">
+      <c r="H11" s="9">
         <v>-3.737352583557367E-2</v>
       </c>
-      <c r="I11" s="6">
+      <c r="I11" s="9">
         <v>0.18187278121709813</v>
       </c>
-      <c r="J11" s="6">
+      <c r="J11" s="9">
         <v>0.49815002351999271</v>
       </c>
-      <c r="K11" s="6">
+      <c r="K11" s="9">
         <v>1.3035588017539313E-3</v>
       </c>
-      <c r="L11" s="6">
+      <c r="L11" s="9">
         <v>3.2569196654064284E-3</v>
       </c>
-      <c r="M11" s="6">
+      <c r="M11" s="9">
         <v>4.1132499928831228E-4</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A12" s="7">
+      <c r="A12" s="4">
         <v>10</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="8">
         <v>0.14714035779858589</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="8">
         <v>6.6978934652676481E-4</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="8">
         <v>0.29300001263618441</v>
       </c>
-      <c r="E12">
+      <c r="E12" s="8">
         <v>2.5006163367234088E-4</v>
       </c>
-      <c r="F12">
+      <c r="F12" s="8">
         <v>4.3760632620160912E-4</v>
       </c>
-      <c r="G12">
+      <c r="G12" s="8">
         <v>3.9061785246932625E-16</v>
       </c>
-      <c r="H12">
+      <c r="H12" s="8">
         <v>-3.1959622962555521E-2</v>
       </c>
-      <c r="I12">
+      <c r="I12" s="8">
         <v>0.18961191689595561</v>
       </c>
-      <c r="J12">
+      <c r="J12" s="8">
         <v>0.8038542059560615</v>
       </c>
-      <c r="K12">
+      <c r="K12" s="8">
         <v>2.287305821937874E-3</v>
       </c>
-      <c r="L12">
+      <c r="L12" s="8">
         <v>2.5588127088746631E-3</v>
       </c>
-      <c r="M12">
+      <c r="M12" s="8">
         <v>9.5123290112216375E-4</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A13" s="7">
+      <c r="A13" s="4">
         <v>11</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="8">
         <v>0.2557120872746913</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="8">
         <v>1.5117761452571191E-2</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="8">
         <v>0.79781654613827335</v>
       </c>
-      <c r="E13">
+      <c r="E13" s="8">
         <v>2.8162487778694446E-3</v>
       </c>
-      <c r="F13">
+      <c r="F13" s="8">
         <v>1.8649319608732187E-3</v>
       </c>
-      <c r="G13">
+      <c r="G13" s="8">
         <v>6.677995366337266E-3</v>
       </c>
-      <c r="H13">
+      <c r="H13" s="8">
         <v>-3.3023906273579359E-2</v>
       </c>
-      <c r="I13">
+      <c r="I13" s="8">
         <v>0.18708912700141223</v>
       </c>
-      <c r="J13">
+      <c r="J13" s="8">
         <v>0.80445875760612129</v>
       </c>
-      <c r="K13">
+      <c r="K13" s="8">
         <v>1.4349099516827635E-3</v>
       </c>
-      <c r="L13">
+      <c r="L13" s="8">
         <v>4.1340654869593142E-3</v>
       </c>
-      <c r="M13">
+      <c r="M13" s="8">
         <v>9.6736784179318367E-4</v>
       </c>
     </row>

</xml_diff>